<commit_message>
Make group numbers more distinguished in template
</commit_message>
<xml_diff>
--- a/our_templates/Our_Template_Efficacy.xlsx
+++ b/our_templates/Our_Template_Efficacy.xlsx
@@ -1392,8 +1392,8 @@
   </sheetPr>
   <dimension ref="A1:S245"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B234" sqref="B234:B245"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="D246" sqref="D246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8124,7 +8124,7 @@
         <v>96</v>
       </c>
       <c r="D128" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E128" s="5" t="s">
         <v>134</v>
@@ -8177,7 +8177,7 @@
         <v>96</v>
       </c>
       <c r="D129" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E129" s="5" t="s">
         <v>135</v>
@@ -8230,7 +8230,7 @@
         <v>96</v>
       </c>
       <c r="D130" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E130" s="5" t="s">
         <v>136</v>
@@ -8283,7 +8283,7 @@
         <v>96</v>
       </c>
       <c r="D131" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E131" s="5" t="s">
         <v>137</v>
@@ -8336,7 +8336,7 @@
         <v>96</v>
       </c>
       <c r="D132" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E132" s="5" t="s">
         <v>138</v>
@@ -8389,7 +8389,7 @@
         <v>96</v>
       </c>
       <c r="D133" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E133" s="5" t="s">
         <v>139</v>
@@ -8442,7 +8442,7 @@
         <v>96</v>
       </c>
       <c r="D134" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E134" s="5" t="s">
         <v>140</v>
@@ -8495,7 +8495,7 @@
         <v>96</v>
       </c>
       <c r="D135" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>141</v>
@@ -8548,7 +8548,7 @@
         <v>145</v>
       </c>
       <c r="D136" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E136" s="5" t="s">
         <v>134</v>
@@ -8601,7 +8601,7 @@
         <v>145</v>
       </c>
       <c r="D137" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E137" s="5" t="s">
         <v>135</v>
@@ -8654,7 +8654,7 @@
         <v>145</v>
       </c>
       <c r="D138" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>136</v>
@@ -8707,7 +8707,7 @@
         <v>145</v>
       </c>
       <c r="D139" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>137</v>
@@ -8760,7 +8760,7 @@
         <v>145</v>
       </c>
       <c r="D140" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E140" s="5" t="s">
         <v>138</v>
@@ -8813,7 +8813,7 @@
         <v>145</v>
       </c>
       <c r="D141" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E141" s="5" t="s">
         <v>139</v>
@@ -8866,7 +8866,7 @@
         <v>145</v>
       </c>
       <c r="D142" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E142" s="5" t="s">
         <v>140</v>
@@ -8919,7 +8919,7 @@
         <v>145</v>
       </c>
       <c r="D143" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>141</v>
@@ -8972,7 +8972,7 @@
         <v>145</v>
       </c>
       <c r="D144" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E144" s="5" t="s">
         <v>142</v>
@@ -9025,7 +9025,7 @@
         <v>145</v>
       </c>
       <c r="D145" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E145" s="5" t="s">
         <v>143</v>
@@ -9078,7 +9078,7 @@
         <v>145</v>
       </c>
       <c r="D146" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E146" s="5" t="s">
         <v>134</v>
@@ -9131,7 +9131,7 @@
         <v>145</v>
       </c>
       <c r="D147" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E147" s="5" t="s">
         <v>135</v>
@@ -9184,7 +9184,7 @@
         <v>145</v>
       </c>
       <c r="D148" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E148" s="5" t="s">
         <v>136</v>
@@ -9237,7 +9237,7 @@
         <v>145</v>
       </c>
       <c r="D149" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E149" s="5" t="s">
         <v>137</v>
@@ -9290,7 +9290,7 @@
         <v>145</v>
       </c>
       <c r="D150" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E150" s="5" t="s">
         <v>138</v>
@@ -9343,7 +9343,7 @@
         <v>145</v>
       </c>
       <c r="D151" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E151" s="5" t="s">
         <v>139</v>
@@ -9396,7 +9396,7 @@
         <v>145</v>
       </c>
       <c r="D152" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E152" s="5" t="s">
         <v>140</v>
@@ -9449,7 +9449,7 @@
         <v>145</v>
       </c>
       <c r="D153" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E153" s="5" t="s">
         <v>141</v>
@@ -9502,7 +9502,7 @@
         <v>145</v>
       </c>
       <c r="D154" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E154" s="5" t="s">
         <v>142</v>
@@ -9555,7 +9555,7 @@
         <v>145</v>
       </c>
       <c r="D155" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E155" s="5" t="s">
         <v>143</v>
@@ -9608,7 +9608,7 @@
         <v>146</v>
       </c>
       <c r="D156" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E156" s="5" t="s">
         <v>134</v>
@@ -9661,7 +9661,7 @@
         <v>146</v>
       </c>
       <c r="D157" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E157" s="5" t="s">
         <v>135</v>
@@ -9714,7 +9714,7 @@
         <v>146</v>
       </c>
       <c r="D158" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E158" s="5" t="s">
         <v>136</v>
@@ -9767,7 +9767,7 @@
         <v>146</v>
       </c>
       <c r="D159" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E159" s="5" t="s">
         <v>137</v>
@@ -9820,7 +9820,7 @@
         <v>146</v>
       </c>
       <c r="D160" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E160" s="5" t="s">
         <v>138</v>
@@ -9873,7 +9873,7 @@
         <v>146</v>
       </c>
       <c r="D161" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E161" s="5" t="s">
         <v>139</v>
@@ -9926,7 +9926,7 @@
         <v>146</v>
       </c>
       <c r="D162" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E162" s="5" t="s">
         <v>140</v>
@@ -9979,7 +9979,7 @@
         <v>146</v>
       </c>
       <c r="D163" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E163" s="5" t="s">
         <v>141</v>
@@ -10032,7 +10032,7 @@
         <v>146</v>
       </c>
       <c r="D164" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E164" s="5" t="s">
         <v>142</v>
@@ -10085,7 +10085,7 @@
         <v>146</v>
       </c>
       <c r="D165" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E165" s="5" t="s">
         <v>143</v>
@@ -10138,7 +10138,7 @@
         <v>147</v>
       </c>
       <c r="D166" s="5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E166" s="5" t="s">
         <v>134</v>
@@ -10191,7 +10191,7 @@
         <v>147</v>
       </c>
       <c r="D167" s="5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E167" s="5" t="s">
         <v>135</v>
@@ -10244,7 +10244,7 @@
         <v>147</v>
       </c>
       <c r="D168" s="5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E168" s="5" t="s">
         <v>136</v>
@@ -10297,7 +10297,7 @@
         <v>147</v>
       </c>
       <c r="D169" s="5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E169" s="5" t="s">
         <v>137</v>
@@ -10350,7 +10350,7 @@
         <v>147</v>
       </c>
       <c r="D170" s="5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E170" s="5" t="s">
         <v>138</v>
@@ -10403,7 +10403,7 @@
         <v>147</v>
       </c>
       <c r="D171" s="5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E171" s="5" t="s">
         <v>139</v>
@@ -10456,7 +10456,7 @@
         <v>147</v>
       </c>
       <c r="D172" s="5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E172" s="5" t="s">
         <v>140</v>
@@ -10509,7 +10509,7 @@
         <v>147</v>
       </c>
       <c r="D173" s="5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E173" s="5" t="s">
         <v>141</v>
@@ -10562,7 +10562,7 @@
         <v>147</v>
       </c>
       <c r="D174" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E174" s="5" t="s">
         <v>142</v>
@@ -10615,7 +10615,7 @@
         <v>147</v>
       </c>
       <c r="D175" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E175" s="5" t="s">
         <v>143</v>
@@ -10668,7 +10668,7 @@
         <v>148</v>
       </c>
       <c r="D176" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E176" s="5" t="s">
         <v>134</v>
@@ -10721,7 +10721,7 @@
         <v>148</v>
       </c>
       <c r="D177" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E177" s="5" t="s">
         <v>135</v>
@@ -10774,7 +10774,7 @@
         <v>148</v>
       </c>
       <c r="D178" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E178" s="5" t="s">
         <v>136</v>
@@ -10827,7 +10827,7 @@
         <v>148</v>
       </c>
       <c r="D179" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E179" s="5" t="s">
         <v>137</v>
@@ -10880,7 +10880,7 @@
         <v>148</v>
       </c>
       <c r="D180" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E180" s="5" t="s">
         <v>138</v>
@@ -10933,7 +10933,7 @@
         <v>148</v>
       </c>
       <c r="D181" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E181" s="5" t="s">
         <v>139</v>
@@ -10986,7 +10986,7 @@
         <v>148</v>
       </c>
       <c r="D182" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E182" s="5" t="s">
         <v>140</v>
@@ -11039,7 +11039,7 @@
         <v>148</v>
       </c>
       <c r="D183" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E183" s="5" t="s">
         <v>141</v>
@@ -11092,7 +11092,7 @@
         <v>148</v>
       </c>
       <c r="D184" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E184" s="5" t="s">
         <v>142</v>
@@ -11145,7 +11145,7 @@
         <v>148</v>
       </c>
       <c r="D185" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E185" s="5" t="s">
         <v>143</v>
@@ -11198,7 +11198,7 @@
         <v>149</v>
       </c>
       <c r="D186" s="5">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E186" s="5" t="s">
         <v>134</v>
@@ -11251,7 +11251,7 @@
         <v>149</v>
       </c>
       <c r="D187" s="5">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E187" s="5" t="s">
         <v>135</v>
@@ -11304,7 +11304,7 @@
         <v>149</v>
       </c>
       <c r="D188" s="5">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E188" s="5" t="s">
         <v>136</v>
@@ -11357,7 +11357,7 @@
         <v>149</v>
       </c>
       <c r="D189" s="5">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E189" s="5" t="s">
         <v>137</v>
@@ -11410,7 +11410,7 @@
         <v>149</v>
       </c>
       <c r="D190" s="5">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E190" s="5" t="s">
         <v>138</v>
@@ -11463,7 +11463,7 @@
         <v>149</v>
       </c>
       <c r="D191" s="5">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E191" s="5" t="s">
         <v>139</v>
@@ -11516,7 +11516,7 @@
         <v>149</v>
       </c>
       <c r="D192" s="5">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E192" s="5" t="s">
         <v>140</v>
@@ -11569,7 +11569,7 @@
         <v>149</v>
       </c>
       <c r="D193" s="5">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E193" s="5" t="s">
         <v>141</v>
@@ -11622,7 +11622,7 @@
         <v>149</v>
       </c>
       <c r="D194" s="5">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E194" s="5" t="s">
         <v>142</v>
@@ -11675,7 +11675,7 @@
         <v>149</v>
       </c>
       <c r="D195" s="5">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E195" s="5" t="s">
         <v>143</v>
@@ -11728,7 +11728,7 @@
         <v>150</v>
       </c>
       <c r="D196" s="5">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E196" s="5" t="s">
         <v>134</v>
@@ -11781,7 +11781,7 @@
         <v>150</v>
       </c>
       <c r="D197" s="5">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E197" s="5" t="s">
         <v>135</v>
@@ -11834,7 +11834,7 @@
         <v>150</v>
       </c>
       <c r="D198" s="5">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E198" s="5" t="s">
         <v>136</v>
@@ -11887,7 +11887,7 @@
         <v>150</v>
       </c>
       <c r="D199" s="5">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E199" s="5" t="s">
         <v>137</v>
@@ -11940,7 +11940,7 @@
         <v>150</v>
       </c>
       <c r="D200" s="5">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E200" s="5" t="s">
         <v>138</v>
@@ -11993,7 +11993,7 @@
         <v>150</v>
       </c>
       <c r="D201" s="5">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E201" s="5" t="s">
         <v>139</v>
@@ -12046,7 +12046,7 @@
         <v>150</v>
       </c>
       <c r="D202" s="5">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E202" s="5" t="s">
         <v>140</v>
@@ -12099,7 +12099,7 @@
         <v>150</v>
       </c>
       <c r="D203" s="5">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E203" s="5" t="s">
         <v>141</v>
@@ -12152,7 +12152,7 @@
         <v>150</v>
       </c>
       <c r="D204" s="5">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E204" s="5" t="s">
         <v>142</v>
@@ -12205,7 +12205,7 @@
         <v>150</v>
       </c>
       <c r="D205" s="5">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E205" s="5" t="s">
         <v>143</v>
@@ -12258,7 +12258,7 @@
         <v>151</v>
       </c>
       <c r="D206" s="5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E206" s="5" t="s">
         <v>134</v>
@@ -12307,7 +12307,7 @@
         <v>151</v>
       </c>
       <c r="D207" s="5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E207" s="5" t="s">
         <v>135</v>
@@ -12356,7 +12356,7 @@
         <v>151</v>
       </c>
       <c r="D208" s="5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E208" s="5" t="s">
         <v>136</v>
@@ -12405,7 +12405,7 @@
         <v>151</v>
       </c>
       <c r="D209" s="5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E209" s="5" t="s">
         <v>137</v>
@@ -12454,7 +12454,7 @@
         <v>151</v>
       </c>
       <c r="D210" s="5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E210" s="5" t="s">
         <v>138</v>
@@ -12503,7 +12503,7 @@
         <v>151</v>
       </c>
       <c r="D211" s="5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E211" s="5" t="s">
         <v>139</v>
@@ -12552,7 +12552,7 @@
         <v>151</v>
       </c>
       <c r="D212" s="5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E212" s="5" t="s">
         <v>140</v>
@@ -12601,7 +12601,7 @@
         <v>151</v>
       </c>
       <c r="D213" s="5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E213" s="5" t="s">
         <v>141</v>
@@ -12650,7 +12650,7 @@
         <v>151</v>
       </c>
       <c r="D214" s="5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E214" s="5" t="s">
         <v>142</v>
@@ -12699,7 +12699,7 @@
         <v>151</v>
       </c>
       <c r="D215" s="5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E215" s="5" t="s">
         <v>143</v>
@@ -12748,7 +12748,7 @@
         <v>152</v>
       </c>
       <c r="D216" s="5">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E216" s="5" t="s">
         <v>134</v>
@@ -12801,7 +12801,7 @@
         <v>152</v>
       </c>
       <c r="D217" s="5">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E217" s="5" t="s">
         <v>135</v>
@@ -12854,7 +12854,7 @@
         <v>152</v>
       </c>
       <c r="D218" s="5">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E218" s="5" t="s">
         <v>136</v>
@@ -12907,7 +12907,7 @@
         <v>152</v>
       </c>
       <c r="D219" s="5">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E219" s="5" t="s">
         <v>137</v>
@@ -12960,7 +12960,7 @@
         <v>152</v>
       </c>
       <c r="D220" s="5">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E220" s="5" t="s">
         <v>138</v>
@@ -13013,7 +13013,7 @@
         <v>152</v>
       </c>
       <c r="D221" s="5">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E221" s="5" t="s">
         <v>139</v>
@@ -13066,7 +13066,7 @@
         <v>152</v>
       </c>
       <c r="D222" s="5">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E222" s="5" t="s">
         <v>140</v>
@@ -13119,7 +13119,7 @@
         <v>152</v>
       </c>
       <c r="D223" s="5">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E223" s="5" t="s">
         <v>141</v>
@@ -13172,7 +13172,7 @@
         <v>152</v>
       </c>
       <c r="D224" s="5">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E224" s="5" t="s">
         <v>142</v>
@@ -13225,7 +13225,7 @@
         <v>152</v>
       </c>
       <c r="D225" s="5">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E225" s="5" t="s">
         <v>143</v>
@@ -13278,7 +13278,7 @@
         <v>153</v>
       </c>
       <c r="D226" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E226" s="5" t="s">
         <v>134</v>
@@ -13331,7 +13331,7 @@
         <v>153</v>
       </c>
       <c r="D227" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E227" s="5" t="s">
         <v>135</v>
@@ -13384,7 +13384,7 @@
         <v>153</v>
       </c>
       <c r="D228" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E228" s="5" t="s">
         <v>136</v>
@@ -13437,7 +13437,7 @@
         <v>153</v>
       </c>
       <c r="D229" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E229" s="5" t="s">
         <v>137</v>
@@ -13490,7 +13490,7 @@
         <v>153</v>
       </c>
       <c r="D230" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E230" s="5" t="s">
         <v>138</v>
@@ -13543,7 +13543,7 @@
         <v>153</v>
       </c>
       <c r="D231" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E231" s="5" t="s">
         <v>139</v>
@@ -13596,7 +13596,7 @@
         <v>153</v>
       </c>
       <c r="D232" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E232" s="5" t="s">
         <v>140</v>
@@ -13649,7 +13649,7 @@
         <v>153</v>
       </c>
       <c r="D233" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E233" s="5" t="s">
         <v>141</v>
@@ -13702,7 +13702,7 @@
         <v>153</v>
       </c>
       <c r="D234" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E234" s="5" t="s">
         <v>142</v>
@@ -13755,7 +13755,7 @@
         <v>153</v>
       </c>
       <c r="D235" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E235" s="5" t="s">
         <v>143</v>
@@ -13808,7 +13808,7 @@
         <v>154</v>
       </c>
       <c r="D236" s="5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E236" s="5" t="s">
         <v>134</v>
@@ -13861,7 +13861,7 @@
         <v>154</v>
       </c>
       <c r="D237" s="5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E237" s="5" t="s">
         <v>135</v>
@@ -13914,7 +13914,7 @@
         <v>154</v>
       </c>
       <c r="D238" s="5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E238" s="5" t="s">
         <v>136</v>
@@ -13967,7 +13967,7 @@
         <v>154</v>
       </c>
       <c r="D239" s="5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E239" s="5" t="s">
         <v>137</v>
@@ -14020,7 +14020,7 @@
         <v>154</v>
       </c>
       <c r="D240" s="5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E240" s="5" t="s">
         <v>138</v>
@@ -14073,7 +14073,7 @@
         <v>154</v>
       </c>
       <c r="D241" s="5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E241" s="5" t="s">
         <v>139</v>
@@ -14126,7 +14126,7 @@
         <v>154</v>
       </c>
       <c r="D242" s="5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E242" s="5" t="s">
         <v>140</v>
@@ -14179,7 +14179,7 @@
         <v>154</v>
       </c>
       <c r="D243" s="5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E243" s="5" t="s">
         <v>141</v>
@@ -14232,7 +14232,7 @@
         <v>154</v>
       </c>
       <c r="D244" s="5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E244" s="5" t="s">
         <v>142</v>
@@ -14285,7 +14285,7 @@
         <v>154</v>
       </c>
       <c r="D245" s="5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E245" s="5" t="s">
         <v>143</v>

</xml_diff>

<commit_message>
Make some adjustments to fix our templates
</commit_message>
<xml_diff>
--- a/our_templates/Our_Template_Efficacy.xlsx
+++ b/our_templates/Our_Template_Efficacy.xlsx
@@ -1379,7 +1379,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1392,8 +1392,8 @@
   </sheetPr>
   <dimension ref="A1:S245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="D246" sqref="D246"/>
+    <sheetView tabSelected="1" topLeftCell="B80" workbookViewId="0">
+      <selection activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6540,7 +6540,7 @@
         <v>134</v>
       </c>
       <c r="F98" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G98" s="5" t="s">
         <v>19</v>
@@ -6549,7 +6549,7 @@
         <v>130</v>
       </c>
       <c r="I98" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J98" s="5">
         <v>20</v>
@@ -6593,7 +6593,7 @@
         <v>135</v>
       </c>
       <c r="F99" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G99" s="5" t="s">
         <v>19</v>
@@ -6602,7 +6602,7 @@
         <v>130</v>
       </c>
       <c r="I99" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J99" s="5">
         <v>20</v>
@@ -6646,7 +6646,7 @@
         <v>136</v>
       </c>
       <c r="F100" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G100" s="5" t="s">
         <v>19</v>
@@ -6655,7 +6655,7 @@
         <v>130</v>
       </c>
       <c r="I100" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J100" s="5">
         <v>20</v>
@@ -6699,7 +6699,7 @@
         <v>137</v>
       </c>
       <c r="F101" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G101" s="5" t="s">
         <v>19</v>
@@ -6708,7 +6708,7 @@
         <v>130</v>
       </c>
       <c r="I101" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J101" s="5">
         <v>20</v>
@@ -6752,7 +6752,7 @@
         <v>138</v>
       </c>
       <c r="F102" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G102" s="5" t="s">
         <v>19</v>
@@ -6761,7 +6761,7 @@
         <v>130</v>
       </c>
       <c r="I102" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J102" s="5">
         <v>20</v>
@@ -6805,7 +6805,7 @@
         <v>139</v>
       </c>
       <c r="F103" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G103" s="5" t="s">
         <v>19</v>
@@ -6814,7 +6814,7 @@
         <v>130</v>
       </c>
       <c r="I103" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J103" s="5">
         <v>20</v>
@@ -6858,7 +6858,7 @@
         <v>140</v>
       </c>
       <c r="F104" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G104" s="5" t="s">
         <v>19</v>
@@ -6867,7 +6867,7 @@
         <v>130</v>
       </c>
       <c r="I104" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J104" s="5">
         <v>20</v>
@@ -6911,7 +6911,7 @@
         <v>141</v>
       </c>
       <c r="F105" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G105" s="5" t="s">
         <v>19</v>
@@ -6920,7 +6920,7 @@
         <v>130</v>
       </c>
       <c r="I105" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J105" s="5">
         <v>20</v>
@@ -6964,7 +6964,7 @@
         <v>142</v>
       </c>
       <c r="F106" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G106" s="5" t="s">
         <v>19</v>
@@ -6973,7 +6973,7 @@
         <v>130</v>
       </c>
       <c r="I106" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J106" s="5">
         <v>20</v>
@@ -7017,7 +7017,7 @@
         <v>143</v>
       </c>
       <c r="F107" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G107" s="5" t="s">
         <v>19</v>
@@ -7026,7 +7026,7 @@
         <v>130</v>
       </c>
       <c r="I107" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J107" s="5">
         <v>20</v>
@@ -7070,7 +7070,7 @@
         <v>134</v>
       </c>
       <c r="F108" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G108" s="5" t="s">
         <v>19</v>
@@ -7079,7 +7079,7 @@
         <v>130</v>
       </c>
       <c r="I108" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J108" s="5">
         <v>20</v>
@@ -7123,7 +7123,7 @@
         <v>135</v>
       </c>
       <c r="F109" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G109" s="5" t="s">
         <v>19</v>
@@ -7132,7 +7132,7 @@
         <v>130</v>
       </c>
       <c r="I109" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J109" s="5">
         <v>20</v>
@@ -7176,7 +7176,7 @@
         <v>136</v>
       </c>
       <c r="F110" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G110" s="5" t="s">
         <v>19</v>
@@ -7185,7 +7185,7 @@
         <v>130</v>
       </c>
       <c r="I110" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J110" s="5">
         <v>20</v>
@@ -7229,7 +7229,7 @@
         <v>137</v>
       </c>
       <c r="F111" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G111" s="5" t="s">
         <v>19</v>
@@ -7238,7 +7238,7 @@
         <v>130</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J111" s="5">
         <v>20</v>
@@ -7282,7 +7282,7 @@
         <v>138</v>
       </c>
       <c r="F112" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G112" s="5" t="s">
         <v>19</v>
@@ -7291,7 +7291,7 @@
         <v>130</v>
       </c>
       <c r="I112" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J112" s="5">
         <v>20</v>
@@ -7335,7 +7335,7 @@
         <v>139</v>
       </c>
       <c r="F113" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G113" s="5" t="s">
         <v>19</v>
@@ -7344,7 +7344,7 @@
         <v>130</v>
       </c>
       <c r="I113" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J113" s="5">
         <v>20</v>
@@ -7388,7 +7388,7 @@
         <v>140</v>
       </c>
       <c r="F114" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G114" s="5" t="s">
         <v>19</v>
@@ -7397,7 +7397,7 @@
         <v>130</v>
       </c>
       <c r="I114" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J114" s="5">
         <v>20</v>
@@ -7441,7 +7441,7 @@
         <v>141</v>
       </c>
       <c r="F115" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G115" s="5" t="s">
         <v>19</v>
@@ -7450,7 +7450,7 @@
         <v>130</v>
       </c>
       <c r="I115" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J115" s="5">
         <v>20</v>
@@ -7494,7 +7494,7 @@
         <v>142</v>
       </c>
       <c r="F116" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G116" s="5" t="s">
         <v>19</v>
@@ -7503,7 +7503,7 @@
         <v>130</v>
       </c>
       <c r="I116" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J116" s="5">
         <v>20</v>
@@ -7547,7 +7547,7 @@
         <v>143</v>
       </c>
       <c r="F117" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G117" s="5" t="s">
         <v>19</v>
@@ -7556,7 +7556,7 @@
         <v>130</v>
       </c>
       <c r="I117" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J117" s="5">
         <v>20</v>
@@ -7600,7 +7600,7 @@
         <v>134</v>
       </c>
       <c r="F118" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G118" s="5" t="s">
         <v>19</v>
@@ -7609,7 +7609,7 @@
         <v>130</v>
       </c>
       <c r="I118" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J118" s="5">
         <v>20</v>
@@ -7653,7 +7653,7 @@
         <v>135</v>
       </c>
       <c r="F119" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G119" s="5" t="s">
         <v>19</v>
@@ -7662,7 +7662,7 @@
         <v>130</v>
       </c>
       <c r="I119" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J119" s="5">
         <v>20</v>
@@ -7706,7 +7706,7 @@
         <v>136</v>
       </c>
       <c r="F120" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G120" s="5" t="s">
         <v>19</v>
@@ -7715,7 +7715,7 @@
         <v>130</v>
       </c>
       <c r="I120" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J120" s="5">
         <v>20</v>
@@ -7759,7 +7759,7 @@
         <v>137</v>
       </c>
       <c r="F121" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G121" s="5" t="s">
         <v>19</v>
@@ -7768,7 +7768,7 @@
         <v>130</v>
       </c>
       <c r="I121" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J121" s="5">
         <v>20</v>
@@ -7812,7 +7812,7 @@
         <v>138</v>
       </c>
       <c r="F122" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G122" s="5" t="s">
         <v>19</v>
@@ -7821,7 +7821,7 @@
         <v>130</v>
       </c>
       <c r="I122" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J122" s="5">
         <v>20</v>
@@ -7865,7 +7865,7 @@
         <v>139</v>
       </c>
       <c r="F123" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G123" s="5" t="s">
         <v>19</v>
@@ -7874,7 +7874,7 @@
         <v>130</v>
       </c>
       <c r="I123" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J123" s="5">
         <v>20</v>
@@ -7918,7 +7918,7 @@
         <v>140</v>
       </c>
       <c r="F124" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G124" s="5" t="s">
         <v>19</v>
@@ -7927,7 +7927,7 @@
         <v>130</v>
       </c>
       <c r="I124" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J124" s="5">
         <v>20</v>
@@ -7971,7 +7971,7 @@
         <v>141</v>
       </c>
       <c r="F125" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G125" s="5" t="s">
         <v>19</v>
@@ -7980,7 +7980,7 @@
         <v>130</v>
       </c>
       <c r="I125" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J125" s="5">
         <v>20</v>
@@ -8024,7 +8024,7 @@
         <v>142</v>
       </c>
       <c r="F126" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G126" s="5" t="s">
         <v>19</v>
@@ -8033,7 +8033,7 @@
         <v>130</v>
       </c>
       <c r="I126" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J126" s="5">
         <v>20</v>
@@ -8077,7 +8077,7 @@
         <v>143</v>
       </c>
       <c r="F127" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G127" s="5" t="s">
         <v>19</v>
@@ -8086,7 +8086,7 @@
         <v>130</v>
       </c>
       <c r="I127" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="J127" s="5">
         <v>20</v>

</xml_diff>